<commit_message>
more harmonization of publisher names
</commit_message>
<xml_diff>
--- a/Data/04_publishers.xlsx
+++ b/Data/04_publishers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e80c4cc3a33b71a/2020 Research/2020-07 Largest Academic Publishers/Academic Publishers and Scholarly Journals/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{EA6F0242-E66E-4FD7-AF08-73D570C04513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2C06B3D-2CA2-4D56-B4AC-581BC572D985}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{EA6F0242-E66E-4FD7-AF08-73D570C04513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF5B8FE8-F282-4D3B-A374-04D6DE470345}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4450,8 +4450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X409"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>